<commit_message>
updating requests to python
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1c74\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moshack_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FB35D8B-5B78-4D42-A5AB-83D7FA4BC068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFA168C-17D8-4E58-8116-2C357FE36C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
   <si>
     <t>Адрес</t>
   </si>
@@ -96,13 +96,16 @@
   </si>
   <si>
     <t>Современная отделка</t>
+  </si>
+  <si>
+    <t>Москва, Ленинские горы, Д. 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,25 +418,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -503,7 +506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -535,6 +538,461 @@
         <v>2800</v>
       </c>
       <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4">
+        <v>2800</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <v>2800</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <v>2800</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>2800</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>2800</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9">
+        <v>2800</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10">
+        <v>2800</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>2800</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12">
+        <v>2800</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>2800</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14">
+        <v>2800</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15">
+        <v>2800</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16">
+        <v>2800</v>
+      </c>
+      <c r="K16" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>